<commit_message>
First attempt to merge Barcelona and Oxford data (with mild success)
</commit_message>
<xml_diff>
--- a/Stimuli/stimuli.xlsx
+++ b/Stimuli/stimuli.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gonza\Documents\CognatePriming\Stimuli\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gonza\Documents\cognate-priming\Stimuli\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A0785D1-CDBE-4D02-AC6F-0C17DE19F30C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B72D9FE8-3DD7-4D62-89A0-8494E219406C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-228" yWindow="12852" windowWidth="23256" windowHeight="12720" xr2:uid="{50B23307-7EAA-A04A-B04A-4FFB3EAC0B6E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{50B23307-7EAA-A04A-B04A-4FFB3EAC0B6E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1695,7 +1695,7 @@
   <dimension ref="A1:S641"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="87" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A638" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A542" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="I267" sqref="I267"/>
     </sheetView>
   </sheetViews>

</xml_diff>